<commit_message>
Writing the detaild for side menu collapsed view, into file for further usability
</commit_message>
<xml_diff>
--- a/yt_multi_language_ui_validator/src/main/resources/data/ExpectedDataGlobalForEnglish.xlsx
+++ b/yt_multi_language_ui_validator/src/main/resources/data/ExpectedDataGlobalForEnglish.xlsx
@@ -8,54 +8,220 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sagar\youtube-multi-language-ui-validator-automation\yt_multi_language_ui_validator\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAE128B-6C71-480E-89BE-AF05DEC74B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02164BC-BF1E-4950-AC6D-800E0FFD8C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>SidemenuCollapsed</t>
-  </si>
-  <si>
-    <t>SidemenuExpanded</t>
-  </si>
-  <si>
-    <t>HomeShortsSubscriptionsYou</t>
-  </si>
-  <si>
-    <t>HomeShortsSubscriptionsYouHistoryShoppingMusicMoviesLiveGamingNewsSportsCoursesFashion&amp;Beauty</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+  <si>
+    <t xml:space="preserve">Tuis Kortvideo's Intekeninge Myne </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ev Shorts Abunəliklər Siz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beranda Shorts Subscription Anda </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Početna stranica Shorts Pretplate Vi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inici YouTube Shorts Subscripcions Tu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start Shorts Abonnementer Dig </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Startseite Shorts Abos Mein YouTube </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avaleht Shorts Tellimused Teie </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Shorts Subscriptions You </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inicio Shorts Suscripciones Tú </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Principal Shorts Suscripciones Tú </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orri nagusia Shorts Harpidetzak Zu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accueil Shorts Abonnements Vous </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Početna Shorts Pretplate Moje </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heim Shorts Áskriftir Þú </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Shorts Iscrizioni Tu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sākums Shorts Abonementi Jūs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pagrindinis Shorts Prenumeratos Jūs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kezdőlap Shorts Feliratkozások Te </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Shorts Abonnementen Jij </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Główna Shorts Subskrypcje Ty </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Início Shorts Subscrições Eu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Início Shorts Inscrições Você </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faqja e parë Shorts Abonimet Ti </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domača stran Kratki videoposnetki Naročnine Vi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Koti Shorts Tilaukset Sinä </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hem Shorts Prenumerationer Ditt YouTube </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trang chủ Shorts Kênh đăng ký Bạn </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ana Sayfa Shorts Abonelikler Siz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Галоўная старонка Shorts Падпіскі Вы </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Начало Shorts Абонаменти Вие </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Главная Shorts Подписки Вы </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Головна YouTube Shorts Підписки Ви </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Αρχική Shorts Εγγραφές Εσείς </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Սկիզբ Shorts Հետևում եմ Դուք </t>
+  </si>
+  <si>
+    <t xml:space="preserve">דף הבית Shorts מינויים הדף שלי </t>
+  </si>
+  <si>
+    <t xml:space="preserve">الصفحة الرئيسية Shorts الاشتراكات أنت </t>
+  </si>
+  <si>
+    <t xml:space="preserve">صفحه اصلی کوته‌ویدیوهای YouTube اشتراک‌ها شما </t>
+  </si>
+  <si>
+    <t xml:space="preserve">होम पेज Shorts सदस्यता आप </t>
+  </si>
+  <si>
+    <t xml:space="preserve">হোম Shorts সাবস্ক্রিপশন আপনি </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਹੋਮ Shorts ਸਬਸਕ੍ਰਿਪਸ਼ਨਾਂ ਤੁਸੀਂ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">હોમ Shorts સબ્સ્ક્રિપ્શન તમે </t>
+  </si>
+  <si>
+    <t xml:space="preserve">முகப்பு Shorts சந்தாக்கள் நீங்கள் </t>
+  </si>
+  <si>
+    <t xml:space="preserve">మొదటి ట్యాబ్ Shorts సబ్‌స్క్రిప్షన్‌లు ఖాతా </t>
+  </si>
+  <si>
+    <t xml:space="preserve">首页 Shorts 订阅 我 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">首頁 Shorts 訂閱內容 個人中心 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">主頁 Shorts 訂閱項目 個人中心 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ホーム ショート 登録チャンネル マイページ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">홈 Shorts 구독 내 페이지 </t>
+  </si>
+  <si>
+    <t>SidemenuCollapsedAppliedLanguage</t>
+  </si>
+  <si>
+    <t>SidemenuCollapsedData</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color theme="1"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,9 +244,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -361,32 +526,293 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" customWidth="1"/>
     <col min="2" max="2" width="77.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="e" cm="1">
+        <f t="array" ref="A2">+A31B1A2:A39A2:A35B1A2A2:A38</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>